<commit_message>
Portraits of the Rim 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Portraits of the Rim - 2937991425/Portraits of the Rim - 2937991425.xlsx
+++ b/Data/Portraits of the Rim - 2937991425/Portraits of the Rim - 2937991425.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\trans\Portraits of the Rim - 2937991425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E73655-F2EC-4A0B-9E84-55C99091AEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A939E308-6458-47B4-9308-958951034FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="7200" windowWidth="28725" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -181,12 +181,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-05-25에 새로 추가된 노드들 (1개)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -215,6 +228,9 @@
     <t>PR.ShowBandagesInsteadOfInjuries</t>
   </si>
   <si>
+    <t>Show bandages instead of injuries</t>
+  </si>
+  <si>
     <t>부상 대신 붕대 표시</t>
   </si>
   <si>
@@ -224,6 +240,9 @@
     <t>PR.RandomizeFaceAndHairAssetsInPlaceOfMissingAssets</t>
   </si>
   <si>
+    <t>Randomize face and hair assets in place of missing assets</t>
+  </si>
+  <si>
     <t>누락된 에셋 대신 얼굴 및 헤어 에셋 무작위 생성</t>
   </si>
   <si>
@@ -233,6 +252,9 @@
     <t>PR.ShowPortraitsByDefault</t>
   </si>
   <si>
+    <t>Show Portraits by default (Toggling this in the main menu may reset all individual portrait show/hide settings)</t>
+  </si>
+  <si>
     <t>인물 사진은 기본적으로 표시됩니다(메인 메뉴에서 이 설정을 토글하면 모든 개별 인물 사진 표시/숨기기 설정이 초기화될 수 있습니다).</t>
   </si>
   <si>
@@ -242,6 +264,9 @@
     <t>PR.HidePortrait</t>
   </si>
   <si>
+    <t>Hide portrait</t>
+  </si>
+  <si>
     <t>초상화 숨기기</t>
   </si>
   <si>
@@ -251,6 +276,9 @@
     <t>PR.ShowPortrait</t>
   </si>
   <si>
+    <t>Show portrait</t>
+  </si>
+  <si>
     <t>초상화 표시</t>
   </si>
   <si>
@@ -260,6 +288,9 @@
     <t>PR.HideHeadgear</t>
   </si>
   <si>
+    <t>Hide headgear</t>
+  </si>
+  <si>
     <t>머리 장식 숨기기</t>
   </si>
   <si>
@@ -269,6 +300,9 @@
     <t>PR.ShowHeadgear</t>
   </si>
   <si>
+    <t>Show headgear</t>
+  </si>
+  <si>
     <t>머리 장식 표시</t>
   </si>
   <si>
@@ -278,6 +312,9 @@
     <t>PR.SelectStyle</t>
   </si>
   <si>
+    <t>Select style</t>
+  </si>
+  <si>
     <t>스타일 선택</t>
   </si>
   <si>
@@ -287,6 +324,9 @@
     <t>PR.SelectExpressedTrait</t>
   </si>
   <si>
+    <t>Select expressed trait</t>
+  </si>
+  <si>
     <t>표현할 특성 선택</t>
   </si>
   <si>
@@ -296,6 +336,9 @@
     <t>PR.NoExpressableTraitNoRandom</t>
   </si>
   <si>
+    <t>Pawn has no expressable trait</t>
+  </si>
+  <si>
     <t>이 폰은 표현 가능한 특성이 없습니다.</t>
   </si>
   <si>
@@ -305,42 +348,12 @@
     <t>PR.NoExpressableTraitRandom</t>
   </si>
   <si>
+    <t>Reroll random face (No expressable trait found on pawn)</t>
+  </si>
+  <si>
     <t>랜덤 얼굴 리롤(표현 가능한 특성 없음)</t>
   </si>
   <si>
-    <t>Show bandages instead of injuries</t>
-  </si>
-  <si>
-    <t>Randomize face and hair assets in place of missing assets</t>
-  </si>
-  <si>
-    <t>Show Portraits by default (Toggling this in the main menu may reset all individual portrait show/hide settings)</t>
-  </si>
-  <si>
-    <t>Hide portrait</t>
-  </si>
-  <si>
-    <t>Show portrait</t>
-  </si>
-  <si>
-    <t>Hide headgear</t>
-  </si>
-  <si>
-    <t>Show headgear</t>
-  </si>
-  <si>
-    <t>Select style</t>
-  </si>
-  <si>
-    <t>Select expressed trait</t>
-  </si>
-  <si>
-    <t>Pawn has no expressable trait</t>
-  </si>
-  <si>
-    <t>Reroll random face (No expressable trait found on pawn)</t>
-  </si>
-  <si>
     <t>Keyed+PR.ShowHeadgearByDefault</t>
   </si>
   <si>
@@ -353,6 +366,18 @@
     <t>Keyed+PR.ShowHeadgearWhenDrafted</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>기본적으로 머리장비 표시 (기존 폰은 개별 토글이 필요할 수 있음)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PR.ShowHeadgearWhenDrafted</t>
   </si>
   <si>
@@ -362,12 +387,27 @@
     <t>Keyed+PR.ReRandomizeHair</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>소집 시 항상 머리장비를 표시합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PR.ReRandomizeHair</t>
   </si>
   <si>
     <t>Reroll randomly selected missing hair asset</t>
   </si>
   <si>
+    <t>누락된 머리 에셋 무작위 선택 리롤</t>
+  </si>
+  <si>
     <t>Keyed+PR.FallbackBaselinerHead</t>
   </si>
   <si>
@@ -377,18 +417,20 @@
     <t>Show default Baseliner head in place of missing heads</t>
   </si>
   <si>
-    <t>기본적으로 머리장비 표시 (기존 폰은 개별 토글이 필요할 수 있음)</t>
+    <t>누락된 머리 대신 기본 일반인 머리 표시하기</t>
+  </si>
+  <si>
+    <t>Keyed+PR.FallbackBaselinerBody</t>
+  </si>
+  <si>
+    <t>PR.FallbackBaselinerBody</t>
+  </si>
+  <si>
+    <t>Show default Baseliner torso in place of missing torsos</t>
+  </si>
+  <si>
+    <t>누락된 몸 대신 기본 일반인 몸 표시하기</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>소집 시 항상 머리장비를 표시합니다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>누락된 머리 에셋 무작위 선택 리롤</t>
-  </si>
-  <si>
-    <t>누락된 머리 대신 기본 일반인 머리 표시하기</t>
   </si>
 </sst>
 </file>
@@ -758,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -801,180 +843,180 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -991,7 +1033,7 @@
         <v>53</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1002,47 +1044,64 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>